<commit_message>
´avance modelo, semana 2
</commit_message>
<xml_diff>
--- a/Matrices_de_ilustracion.xlsx
+++ b/Matrices_de_ilustracion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Documentos\POD2021\WarehaousingLabEafit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C00143-C3B1-436C-8FFF-343DDBDED04C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E17FC1-E79D-4FE1-8937-9D99B325CEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="990" windowWidth="19875" windowHeight="14610" xr2:uid="{02B89D4E-1FAF-4C94-B2A9-843983FDD318}"/>
   </bookViews>
@@ -34,13 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>conjunto de posiciones  L</t>
-  </si>
-  <si>
-    <t>conjunto de ordenes M</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>conjunto de batches</t>
   </si>
@@ -49,6 +43,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Conjunto posiciones</t>
+  </si>
+  <si>
+    <t>conjunto de ordenes</t>
+  </si>
+  <si>
+    <t>conjunto de posiciones</t>
   </si>
 </sst>
 </file>
@@ -98,14 +98,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F04DDD3-DA0F-4E30-BC2E-40622E3B3420}">
-  <dimension ref="A3:M16"/>
+  <dimension ref="A3:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,24 +433,24 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="H3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
+      <c r="A4" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -464,12 +464,12 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>2</v>
+      <c r="H4" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="I4">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:L15" ca="1" si="0">RANDBETWEEN(0,1)</f>
@@ -477,7 +477,7 @@
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
@@ -485,7 +485,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="4"/>
       <c r="B5">
         <v>0</v>
       </c>
@@ -498,14 +498,14 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="4"/>
       <c r="I5">
         <f t="shared" ref="I5:I15" ca="1" si="1">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
@@ -513,11 +513,11 @@
       </c>
       <c r="L5">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="4"/>
       <c r="B6">
         <v>1</v>
       </c>
@@ -530,7 +530,7 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="4"/>
       <c r="I6">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
@@ -545,11 +545,11 @@
       </c>
       <c r="L6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="4"/>
       <c r="B7">
         <v>0</v>
       </c>
@@ -562,10 +562,10 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="4"/>
       <c r="I7">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
@@ -581,7 +581,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="4"/>
       <c r="B8">
         <v>1</v>
       </c>
@@ -594,7 +594,7 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="4"/>
       <c r="I8">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
@@ -609,11 +609,11 @@
       </c>
       <c r="L8">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="4"/>
       <c r="B9">
         <v>1</v>
       </c>
@@ -626,26 +626,26 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="4"/>
       <c r="I9">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="4"/>
       <c r="B10">
         <v>0</v>
       </c>
@@ -658,7 +658,7 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="4"/>
       <c r="I10">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
@@ -677,7 +677,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="4"/>
       <c r="B11">
         <v>0</v>
       </c>
@@ -690,14 +690,14 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="4"/>
       <c r="I11">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="0"/>
@@ -705,11 +705,11 @@
       </c>
       <c r="L11">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="4"/>
       <c r="B12">
         <v>1</v>
       </c>
@@ -722,18 +722,18 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="4"/>
       <c r="I12">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <f t="shared" ca="1" si="0"/>
@@ -741,7 +741,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="4"/>
       <c r="B13">
         <v>0</v>
       </c>
@@ -754,7 +754,7 @@
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="4"/>
       <c r="I13">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
@@ -773,7 +773,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="4"/>
       <c r="B14">
         <v>1</v>
       </c>
@@ -786,14 +786,14 @@
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="4"/>
       <c r="I14">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="0"/>
@@ -805,7 +805,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="4"/>
       <c r="B15">
         <v>0</v>
       </c>
@@ -818,18 +818,18 @@
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="H15" s="2"/>
+      <c r="H15" s="4"/>
       <c r="I15">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15">
         <f t="shared" ca="1" si="0"/>
@@ -837,52 +837,266 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="3">
+      <c r="B16" s="1">
         <f>SUM(B4:B15)</f>
         <v>5</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="1">
         <f t="shared" ref="C16:E16" si="2">SUM(C4:C15)</f>
         <v>9</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="1">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I16">
         <f ca="1">SUM(I4:I15)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J16">
         <f t="shared" ref="J16:L16" ca="1" si="3">SUM(J4:J15)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L16">
         <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="M16" s="2">
+        <f ca="1">SUM(I16:L16)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <f>SUM(B21:B32)</f>
         <v>5</v>
       </c>
-      <c r="M16" s="4">
-        <f ca="1">SUM(I16:L16)</f>
-        <v>22</v>
+      <c r="C33" s="1">
+        <f t="shared" ref="C33:E33" si="4">SUM(C21:C32)</f>
+        <v>9</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="E33" s="1">
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="A21:A32"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:A15"/>
     <mergeCell ref="H3:L3"/>
     <mergeCell ref="H4:H15"/>
+    <mergeCell ref="A20:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modelo con todas las restricciones
</commit_message>
<xml_diff>
--- a/Matrices_de_ilustracion.xlsx
+++ b/Matrices_de_ilustracion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Documentos\POD2021\WarehaousingLabEafit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BD6F68-4F2E-4391-8A3F-9062F9FFACA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61240E5D-020F-4EBF-BFE3-CAF174500CAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="990" windowWidth="19875" windowHeight="14610" xr2:uid="{02B89D4E-1FAF-4C94-B2A9-843983FDD318}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>conjunto de batches</t>
   </si>
@@ -68,6 +68,15 @@
   <si>
     <t>A,B,C</t>
   </si>
+  <si>
+    <t>Vfj</t>
+  </si>
+  <si>
+    <t>Xij</t>
+  </si>
+  <si>
+    <t>Yfi</t>
+  </si>
 </sst>
 </file>
 
@@ -82,7 +91,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,6 +116,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -237,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -254,6 +269,21 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -281,20 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F04DDD3-DA0F-4E30-BC2E-40622E3B3420}">
   <dimension ref="A2:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,33 +638,40 @@
     <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19"/>
-      <c r="I3" s="22" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+      <c r="I3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="24"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="31"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="22">
         <v>1</v>
       </c>
       <c r="D4" s="8">
@@ -659,12 +683,12 @@
       <c r="F4" s="9">
         <v>1</v>
       </c>
-      <c r="G4" s="30"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="29" t="s">
+      <c r="I4" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="20" t="s">
         <v>10</v>
       </c>
       <c r="K4" s="1">
@@ -673,7 +697,7 @@
       </c>
       <c r="L4" s="1">
         <f t="shared" ref="L4:N15" ca="1" si="0">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -681,12 +705,12 @@
       </c>
       <c r="N4" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="26" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="8">
@@ -701,17 +725,17 @@
       <c r="F5" s="9">
         <v>0</v>
       </c>
-      <c r="G5" s="30"/>
+      <c r="G5" s="21"/>
       <c r="H5" s="15"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="28"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="19"/>
       <c r="K5" s="1">
         <f t="shared" ref="K5:K15" ca="1" si="1">RANDBETWEEN(0,1)</f>
         <v>1</v>
       </c>
       <c r="L5" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -719,15 +743,15 @@
       </c>
       <c r="N5" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="26" t="s">
+      <c r="A6" s="27"/>
+      <c r="B6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="22">
         <v>1</v>
       </c>
       <c r="D6" s="8">
@@ -739,13 +763,13 @@
       <c r="F6" s="9">
         <v>0</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="28"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="19"/>
       <c r="K6" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -753,7 +777,7 @@
       </c>
       <c r="M6" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -761,8 +785,8 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="26" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="8">
@@ -777,30 +801,30 @@
       <c r="F7" s="9">
         <v>0</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="28"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="19"/>
       <c r="K7" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="8">
         <v>1</v>
       </c>
@@ -813,15 +837,15 @@
       <c r="F8" s="9">
         <v>1</v>
       </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="28"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="19"/>
       <c r="K8" s="1">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -833,8 +857,8 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="8">
         <v>1</v>
       </c>
@@ -847,15 +871,15 @@
       <c r="F9" s="9">
         <v>1</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="28"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="19"/>
       <c r="K9" s="1">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -863,12 +887,12 @@
       </c>
       <c r="N9" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="8">
         <v>0</v>
       </c>
@@ -881,15 +905,15 @@
       <c r="F10" s="9">
         <v>1</v>
       </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="28"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="19"/>
       <c r="K10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -901,8 +925,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="26"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="8">
         <v>0</v>
       </c>
@@ -915,8 +939,8 @@
       <c r="F11" s="9">
         <v>1</v>
       </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="28"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="19"/>
       <c r="K11" s="1">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
@@ -935,8 +959,8 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="26"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="8">
         <v>1</v>
       </c>
@@ -949,15 +973,15 @@
       <c r="F12" s="9">
         <v>0</v>
       </c>
-      <c r="I12" s="16"/>
-      <c r="J12" s="28"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="19"/>
       <c r="K12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="1">
         <f t="shared" ca="1" si="0"/>
@@ -969,8 +993,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="8">
         <v>0</v>
       </c>
@@ -983,19 +1007,19 @@
       <c r="F13" s="9">
         <v>0</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="28"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="19"/>
       <c r="K13" s="1">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -1003,8 +1027,8 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="26"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="8">
         <v>1</v>
       </c>
@@ -1017,19 +1041,19 @@
       <c r="F14" s="9">
         <v>1</v>
       </c>
-      <c r="I14" s="16"/>
-      <c r="J14" s="28"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="19"/>
       <c r="K14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="2">
         <f t="shared" ca="1" si="0"/>
@@ -1037,8 +1061,8 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21"/>
-      <c r="B15" s="27"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="10">
         <v>0</v>
       </c>
@@ -1051,23 +1075,23 @@
       <c r="F15" s="11">
         <v>1</v>
       </c>
-      <c r="I15" s="16"/>
-      <c r="J15" s="28"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="19"/>
       <c r="K15" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1095,38 +1119,45 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4">
         <f ca="1">SUM(K4:K15)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L16" s="4">
         <f t="shared" ref="L16:N16" ca="1" si="3">SUM(L4:L15)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M16" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>11</v>
-      </c>
-      <c r="O16" s="15"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+        <v>6</v>
+      </c>
+      <c r="O16" s="32">
+        <f ca="1">SUM(K16:N16)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="24"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="31"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="28"/>
+      <c r="A21" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="19"/>
       <c r="C21" s="1">
         <v>0</v>
       </c>
@@ -1139,13 +1170,13 @@
       <c r="F21" s="2">
         <v>0</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="1">
         <v>0</v>
       </c>
@@ -1158,13 +1189,13 @@
       <c r="F22" s="2">
         <v>0</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="28"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="19"/>
       <c r="C23" s="1">
         <v>1</v>
       </c>
@@ -1182,8 +1213,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="19"/>
       <c r="C24" s="1">
         <v>0</v>
       </c>
@@ -1196,13 +1227,13 @@
       <c r="F24" s="2">
         <v>0</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
-      <c r="B25" s="28"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="1">
         <v>1</v>
       </c>
@@ -1215,13 +1246,13 @@
       <c r="F25" s="2">
         <v>1</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="28"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="19"/>
       <c r="C26" s="1">
         <v>1</v>
       </c>
@@ -1234,13 +1265,13 @@
       <c r="F26" s="2">
         <v>1</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="28"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="1">
         <v>0</v>
       </c>
@@ -1255,8 +1286,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="28"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="19"/>
       <c r="C28" s="1">
         <v>0</v>
       </c>
@@ -1271,8 +1302,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="28"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="19"/>
       <c r="C29" s="1">
         <v>1</v>
       </c>
@@ -1287,8 +1318,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="28"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="19"/>
       <c r="C30" s="1">
         <v>0</v>
       </c>
@@ -1303,8 +1334,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="28"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="19"/>
       <c r="C31" s="1">
         <v>1</v>
       </c>
@@ -1319,8 +1350,8 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="16"/>
-      <c r="B32" s="28"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="19"/>
       <c r="C32" s="1">
         <v>0</v>
       </c>

</xml_diff>